<commit_message>
Finished Repair import data
</commit_message>
<xml_diff>
--- a/wwwroot/uploads/TemplateForm/TemplateMedicalClaim.xlsx
+++ b/wwwroot/uploads/TemplateForm/TemplateMedicalClaim.xlsx
@@ -4,15 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Claim" sheetId="1" r:id="rId1"/>
+    <sheet name="Example" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
@@ -24,7 +23,7 @@
     <author>Tiara</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +75,69 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="0">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Tiara</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tiara:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+CART NAME =
+- RAWAT_JALAN
+- RAWAT_INAP
+- MELAHIRKAN
+- KACAMATA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tiara:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Prd Gajian, sebagai tolak ukur dari rumus status</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>NO</t>
   </si>
@@ -154,6 +215,12 @@
   </si>
   <si>
     <t>Period</t>
+  </si>
+  <si>
+    <t>Kode</t>
+  </si>
+  <si>
+    <t>1234/KS/XI/24</t>
   </si>
 </sst>
 </file>
@@ -225,47 +292,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -36132,65 +36192,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="4" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -36204,68 +36340,39 @@
         <f>VLOOKUP(C2,'[1]Lembar Tugas'!$A$2:$B$1826,2,FALSE)</f>
         <v>DESTIARA KARINI</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="3">
         <f>VLOOKUP(C2,'[1]Lembar Tugas'!$A$2:$F$1826,6,FALSE)</f>
         <v>44714</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="4">
         <v>45605</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="6">
+      <c r="J2" s="6">
         <v>50000</v>
       </c>
-      <c r="J2" s="7">
-        <f>(E2+91)</f>
+      <c r="K2" s="7">
+        <f>(F2+91)</f>
         <v>44805</v>
       </c>
-      <c r="K2" s="8" t="str">
-        <f t="shared" ref="K2" si="0">IF(J2&gt;$L$1,"y","t")</f>
+      <c r="L2" s="8" t="str">
+        <f t="shared" ref="L2" si="0">IF(K2&gt;$M$1,"y","t")</f>
         <v>t</v>
       </c>
-      <c r="L2" s="11">
+      <c r="M2" s="10">
         <v>45627</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>